<commit_message>
Updated YPS Business Plan.docx and YPS Personal Financial Statement.xlsx
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Personal Financial Statement.xlsx
+++ b/Business Plan Documents/YPS Personal Financial Statement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PFS - Dadulla" sheetId="3" r:id="rId1"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="70">
   <si>
     <t>Assets</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Life insurance (cash surrender value)</t>
   </si>
   <si>
-    <t>Personal property (autos, jewelry, etc.)</t>
-  </si>
-  <si>
     <t>Other assets (specify)</t>
   </si>
   <si>
@@ -372,6 +369,32 @@
   </si>
   <si>
     <t>Cash - savings accounts (BPI)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Life insurance (cash surrender value) - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MBAI</t>
+    </r>
+  </si>
+  <si>
+    <t>Personal property (Laptops, desktop, mobile phone)</t>
+  </si>
+  <si>
+    <t>Personal property (Laptop, mobile phone, watches.)</t>
+  </si>
+  <si>
+    <t>Personal property (Laptop, mobile phone, jewelries)</t>
+  </si>
+  <si>
+    <t>Personal property (Laptop, mobile phone, jewelry)</t>
   </si>
 </sst>
 </file>
@@ -502,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -590,13 +613,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -638,6 +655,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1815,22 +1839,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>58</v>
+      <c r="A1" s="50" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+      <c r="A4" s="53">
         <v>42095</v>
       </c>
     </row>
@@ -1848,36 +1872,36 @@
         <v>0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="51">
         <v>40000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="51">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B11" s="1">
         <v>50000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="1">
-        <v>70000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1885,7 +1909,7 @@
     </row>
     <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -1893,31 +1917,31 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>2</v>
+      <c r="A15" s="39" t="s">
+        <v>65</v>
       </c>
       <c r="B15" s="1">
-        <v>120000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
+      <c r="A16" s="39" t="s">
+        <v>66</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -1925,15 +1949,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2000000</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -1941,7 +1963,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1949,32 +1971,32 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="54">
+        <v>4</v>
+      </c>
+      <c r="B21" s="52">
         <f>SUM(B9:B20)</f>
-        <v>2280000</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="56">
+        <v>6</v>
+      </c>
+      <c r="B24" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1982,7 +2004,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1990,7 +2012,7 @@
     </row>
     <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1998,7 +2020,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -2006,7 +2028,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -2014,29 +2036,29 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="57">
+        <v>9</v>
+      </c>
+      <c r="B30" s="55">
         <f>SUM(B24:B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="58">
+        <v>10</v>
+      </c>
+      <c r="B32" s="56">
         <f>(B21-B30)</f>
-        <v>2280000</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2044,21 +2066,21 @@
       <c r="C39" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>19</v>
+      <c r="A41" s="50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
-        <v>28</v>
+      <c r="A44" s="49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -2072,7 +2094,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2086,7 +2108,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2094,25 +2116,25 @@
     </row>
     <row r="50" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="C50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="E50" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="G50" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -2120,14 +2142,14 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="25"/>
-      <c r="B51" s="37">
-        <v>0</v>
-      </c>
-      <c r="C51" s="37">
+      <c r="B51" s="57">
+        <v>0</v>
+      </c>
+      <c r="C51" s="57">
         <v>0</v>
       </c>
       <c r="D51" s="27"/>
-      <c r="E51" s="37">
+      <c r="E51" s="57">
         <v>0</v>
       </c>
       <c r="F51" s="25"/>
@@ -2138,10 +2160,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="25"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="25"/>
-      <c r="E52" s="38"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="3"/>
@@ -2150,10 +2172,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="25"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="25"/>
-      <c r="E53" s="38"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="3"/>
@@ -2162,10 +2184,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="37"/>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="3"/>
@@ -2174,10 +2196,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="25"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="25"/>
-      <c r="E55" s="38"/>
+      <c r="E55" s="37"/>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="3"/>
@@ -2186,10 +2208,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="25"/>
-      <c r="E56" s="38"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="3"/>
@@ -2202,68 +2224,68 @@
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
-        <v>39</v>
+      <c r="A58" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:10" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="C59" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="33" t="s">
+      <c r="E59" s="33" t="s">
         <v>15</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>16</v>
       </c>
       <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="39">
-        <v>0</v>
-      </c>
-      <c r="D60" s="39">
-        <v>0</v>
-      </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="41"/>
+      <c r="C60" s="58">
+        <v>0</v>
+      </c>
+      <c r="D60" s="58">
+        <v>0</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="39"/>
     </row>
     <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
       <c r="B61" s="25"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="25"/>
       <c r="B62" s="25"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
       <c r="B63" s="25"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="25"/>
       <c r="B64" s="25"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2272,33 +2294,33 @@
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="46" t="s">
-        <v>40</v>
+      <c r="A66" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="C67" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="D67" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="25"/>
       <c r="B68" s="35"/>
-      <c r="C68" s="45">
-        <v>0</v>
-      </c>
-      <c r="D68" s="45">
+      <c r="C68" s="59">
+        <v>0</v>
+      </c>
+      <c r="D68" s="59">
         <v>0</v>
       </c>
     </row>
@@ -2328,115 +2350,115 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="12"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="30" t="s">
+      <c r="D74" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>48</v>
       </c>
       <c r="F74" s="21"/>
     </row>
     <row r="75" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="28"/>
-      <c r="B75" s="37">
-        <v>0</v>
-      </c>
-      <c r="C75" s="37">
-        <v>0</v>
-      </c>
-      <c r="D75" s="37">
+      <c r="B75" s="57">
+        <v>0</v>
+      </c>
+      <c r="C75" s="57">
+        <v>0</v>
+      </c>
+      <c r="D75" s="57">
         <v>0</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="27"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="43"/>
+      <c r="G76" s="41"/>
     </row>
     <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="27"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="43"/>
+      <c r="G77" s="41"/>
     </row>
     <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="27"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="43"/>
+      <c r="G78" s="41"/>
     </row>
     <row r="79" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="27"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="43"/>
+      <c r="G79" s="41"/>
     </row>
     <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="43"/>
+      <c r="G80" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="45" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="46" t="s">
         <v>51</v>
-      </c>
-      <c r="B85" s="48" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="25"/>
-      <c r="B86" s="45">
+      <c r="B86" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="25"/>
-      <c r="B87" s="45"/>
+      <c r="B87" s="43"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="25"/>
@@ -2447,146 +2469,146 @@
       <c r="B89" s="36"/>
     </row>
     <row r="91" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="46" t="s">
-        <v>53</v>
+      <c r="A91" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:7" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B92" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="F92" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>56</v>
       </c>
       <c r="G92" s="16"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="25"/>
-      <c r="B93" s="37">
-        <v>0</v>
-      </c>
-      <c r="C93" s="37">
-        <v>0</v>
-      </c>
-      <c r="D93" s="37">
-        <v>0</v>
-      </c>
-      <c r="E93" s="50"/>
+      <c r="B93" s="57">
+        <v>0</v>
+      </c>
+      <c r="C93" s="57">
+        <v>0</v>
+      </c>
+      <c r="D93" s="57">
+        <v>0</v>
+      </c>
+      <c r="E93" s="48"/>
       <c r="F93" s="25"/>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="25"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="50"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="48"/>
       <c r="F94" s="25"/>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="25"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="50"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="48"/>
       <c r="F95" s="25"/>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="25"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="50"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="48"/>
       <c r="F96" s="25"/>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="25"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="50"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="48"/>
       <c r="F97" s="25"/>
       <c r="G97" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
-        <v>57</v>
+      <c r="A99" s="45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E100" s="34" t="s">
+      <c r="F100" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F100" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="25"/>
-      <c r="B101" s="37">
-        <v>0</v>
-      </c>
-      <c r="C101" s="37">
-        <v>0</v>
-      </c>
-      <c r="D101" s="37">
-        <v>0</v>
-      </c>
-      <c r="E101" s="50"/>
+      <c r="B101" s="57">
+        <v>0</v>
+      </c>
+      <c r="C101" s="57">
+        <v>0</v>
+      </c>
+      <c r="D101" s="57">
+        <v>0</v>
+      </c>
+      <c r="E101" s="48"/>
       <c r="F101" s="25"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="25"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="50"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="48"/>
       <c r="F102" s="25"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="25"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="50"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="48"/>
       <c r="F103" s="25"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="25"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="50"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="48"/>
       <c r="F104" s="25"/>
     </row>
   </sheetData>
@@ -2600,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2616,22 +2638,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>58</v>
+      <c r="A1" s="50" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+      <c r="A4" s="53">
         <v>42095</v>
       </c>
     </row>
@@ -2649,36 +2671,36 @@
         <v>0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="53">
-        <v>60000</v>
+      <c r="B9" s="51">
+        <v>50000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="1">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>65</v>
-      </c>
       <c r="B11" s="1">
-        <v>90000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -2686,7 +2708,7 @@
     </row>
     <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -2694,7 +2716,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -2709,16 +2731,16 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
+      <c r="A16" s="39" t="s">
+        <v>67</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -2726,15 +2748,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1500000</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -2742,7 +2762,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -2750,32 +2770,32 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="54">
+        <v>4</v>
+      </c>
+      <c r="B21" s="52">
         <f>SUM(B9:B20)</f>
-        <v>1830000</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="56">
+        <v>6</v>
+      </c>
+      <c r="B24" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -2783,7 +2803,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -2791,7 +2811,7 @@
     </row>
     <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -2799,7 +2819,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -2807,7 +2827,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -2815,29 +2835,29 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="57">
+        <v>9</v>
+      </c>
+      <c r="B30" s="55">
         <f>SUM(B24:B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="58">
+        <v>10</v>
+      </c>
+      <c r="B32" s="56">
         <f>(B21-B30)</f>
-        <v>1830000</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,21 +2865,21 @@
       <c r="C39" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>19</v>
+      <c r="A41" s="50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
-        <v>28</v>
+      <c r="A44" s="49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -2873,7 +2893,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2887,7 +2907,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2895,25 +2915,25 @@
     </row>
     <row r="50" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="C50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="E50" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="G50" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -2921,14 +2941,14 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="25"/>
-      <c r="B51" s="37">
-        <v>0</v>
-      </c>
-      <c r="C51" s="37">
+      <c r="B51" s="57">
+        <v>0</v>
+      </c>
+      <c r="C51" s="57">
         <v>0</v>
       </c>
       <c r="D51" s="27"/>
-      <c r="E51" s="37">
+      <c r="E51" s="57">
         <v>0</v>
       </c>
       <c r="F51" s="25"/>
@@ -2939,10 +2959,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="25"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="25"/>
-      <c r="E52" s="38"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="3"/>
@@ -2951,10 +2971,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="25"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="25"/>
-      <c r="E53" s="38"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="3"/>
@@ -2963,10 +2983,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="37"/>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="3"/>
@@ -2975,10 +2995,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="25"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="25"/>
-      <c r="E55" s="38"/>
+      <c r="E55" s="37"/>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="3"/>
@@ -2987,10 +3007,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="25"/>
-      <c r="E56" s="38"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="3"/>
@@ -3003,68 +3023,68 @@
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
-        <v>39</v>
+      <c r="A58" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:10" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="C59" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="33" t="s">
+      <c r="E59" s="33" t="s">
         <v>15</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>16</v>
       </c>
       <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="39">
-        <v>0</v>
-      </c>
-      <c r="D60" s="39">
-        <v>0</v>
-      </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="41"/>
+      <c r="C60" s="58">
+        <v>0</v>
+      </c>
+      <c r="D60" s="58">
+        <v>0</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="39"/>
     </row>
     <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
       <c r="B61" s="25"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="25"/>
       <c r="B62" s="25"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
       <c r="B63" s="25"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="25"/>
       <c r="B64" s="25"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3073,33 +3093,33 @@
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="46" t="s">
-        <v>40</v>
+      <c r="A66" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="C67" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="D67" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="25"/>
       <c r="B68" s="35"/>
-      <c r="C68" s="45">
-        <v>0</v>
-      </c>
-      <c r="D68" s="45">
+      <c r="C68" s="59">
+        <v>0</v>
+      </c>
+      <c r="D68" s="59">
         <v>0</v>
       </c>
     </row>
@@ -3129,115 +3149,115 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="12"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="30" t="s">
+      <c r="D74" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>48</v>
       </c>
       <c r="F74" s="21"/>
     </row>
     <row r="75" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="28"/>
-      <c r="B75" s="37">
-        <v>0</v>
-      </c>
-      <c r="C75" s="37">
-        <v>0</v>
-      </c>
-      <c r="D75" s="37">
+      <c r="B75" s="57">
+        <v>0</v>
+      </c>
+      <c r="C75" s="57">
+        <v>0</v>
+      </c>
+      <c r="D75" s="57">
         <v>0</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="27"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="43"/>
+      <c r="G76" s="41"/>
     </row>
     <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="27"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="43"/>
+      <c r="G77" s="41"/>
     </row>
     <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="27"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="43"/>
+      <c r="G78" s="41"/>
     </row>
     <row r="79" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="27"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="43"/>
+      <c r="G79" s="41"/>
     </row>
     <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="43"/>
+      <c r="G80" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="45" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="46" t="s">
         <v>51</v>
-      </c>
-      <c r="B85" s="48" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="25"/>
-      <c r="B86" s="45">
+      <c r="B86" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="25"/>
-      <c r="B87" s="45"/>
+      <c r="B87" s="43"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="25"/>
@@ -3248,146 +3268,146 @@
       <c r="B89" s="36"/>
     </row>
     <row r="91" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="46" t="s">
-        <v>53</v>
+      <c r="A91" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:7" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B92" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="F92" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>56</v>
       </c>
       <c r="G92" s="16"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="25"/>
-      <c r="B93" s="37">
-        <v>0</v>
-      </c>
-      <c r="C93" s="37">
-        <v>0</v>
-      </c>
-      <c r="D93" s="37">
-        <v>0</v>
-      </c>
-      <c r="E93" s="50"/>
+      <c r="B93" s="57">
+        <v>0</v>
+      </c>
+      <c r="C93" s="57">
+        <v>0</v>
+      </c>
+      <c r="D93" s="57">
+        <v>0</v>
+      </c>
+      <c r="E93" s="48"/>
       <c r="F93" s="25"/>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="25"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="50"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="48"/>
       <c r="F94" s="25"/>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="25"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="50"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="48"/>
       <c r="F95" s="25"/>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="25"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="50"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="48"/>
       <c r="F96" s="25"/>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="25"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="50"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="48"/>
       <c r="F97" s="25"/>
       <c r="G97" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
-        <v>57</v>
+      <c r="A99" s="45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E100" s="34" t="s">
+      <c r="F100" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F100" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="25"/>
-      <c r="B101" s="37">
-        <v>0</v>
-      </c>
-      <c r="C101" s="37">
-        <v>0</v>
-      </c>
-      <c r="D101" s="37">
-        <v>0</v>
-      </c>
-      <c r="E101" s="50"/>
+      <c r="B101" s="57">
+        <v>0</v>
+      </c>
+      <c r="C101" s="57">
+        <v>0</v>
+      </c>
+      <c r="D101" s="57">
+        <v>0</v>
+      </c>
+      <c r="E101" s="48"/>
       <c r="F101" s="25"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="25"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="50"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="48"/>
       <c r="F102" s="25"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="25"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="50"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="48"/>
       <c r="F103" s="25"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="25"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="50"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="48"/>
       <c r="F104" s="25"/>
     </row>
   </sheetData>
@@ -3404,8 +3424,8 @@
   </sheetPr>
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3420,22 +3440,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>58</v>
+      <c r="A1" s="50" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+      <c r="A4" s="53">
         <v>42095</v>
       </c>
     </row>
@@ -3453,36 +3473,36 @@
         <v>0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="51">
         <v>50000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="51">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="53">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>65</v>
-      </c>
       <c r="B11" s="1">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -3490,7 +3510,7 @@
     </row>
     <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -3498,7 +3518,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -3513,16 +3533,16 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
+      <c r="A16" s="39" t="s">
+        <v>68</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -3530,15 +3550,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1500000</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -3546,7 +3564,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -3554,32 +3572,32 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="54">
+        <v>4</v>
+      </c>
+      <c r="B21" s="52">
         <f>SUM(B9:B20)</f>
-        <v>1700000</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="56">
+        <v>6</v>
+      </c>
+      <c r="B24" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -3587,7 +3605,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -3595,7 +3613,7 @@
     </row>
     <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -3603,7 +3621,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -3611,7 +3629,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -3619,29 +3637,29 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="57">
+        <v>9</v>
+      </c>
+      <c r="B30" s="55">
         <f>SUM(B24:B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="58">
+        <v>10</v>
+      </c>
+      <c r="B32" s="56">
         <f>(B21-B30)</f>
-        <v>1700000</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3649,21 +3667,21 @@
       <c r="C39" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>19</v>
+      <c r="A41" s="50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
-        <v>28</v>
+      <c r="A44" s="49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -3677,7 +3695,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3691,7 +3709,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3699,25 +3717,25 @@
     </row>
     <row r="50" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="C50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="E50" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="G50" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -3725,14 +3743,14 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="25"/>
-      <c r="B51" s="37">
-        <v>0</v>
-      </c>
-      <c r="C51" s="37">
+      <c r="B51" s="57">
+        <v>0</v>
+      </c>
+      <c r="C51" s="57">
         <v>0</v>
       </c>
       <c r="D51" s="27"/>
-      <c r="E51" s="37">
+      <c r="E51" s="57">
         <v>0</v>
       </c>
       <c r="F51" s="25"/>
@@ -3743,10 +3761,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="25"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="25"/>
-      <c r="E52" s="38"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="3"/>
@@ -3755,10 +3773,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="25"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="25"/>
-      <c r="E53" s="38"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="3"/>
@@ -3767,10 +3785,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="37"/>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="3"/>
@@ -3779,10 +3797,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="25"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="25"/>
-      <c r="E55" s="38"/>
+      <c r="E55" s="37"/>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="3"/>
@@ -3791,10 +3809,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="25"/>
-      <c r="E56" s="38"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="3"/>
@@ -3807,68 +3825,68 @@
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
-        <v>39</v>
+      <c r="A58" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:10" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="C59" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="33" t="s">
+      <c r="E59" s="33" t="s">
         <v>15</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>16</v>
       </c>
       <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="39">
-        <v>0</v>
-      </c>
-      <c r="D60" s="39">
-        <v>0</v>
-      </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="41"/>
+      <c r="C60" s="58">
+        <v>0</v>
+      </c>
+      <c r="D60" s="58">
+        <v>0</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="39"/>
     </row>
     <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
       <c r="B61" s="25"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="25"/>
       <c r="B62" s="25"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
       <c r="B63" s="25"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="25"/>
       <c r="B64" s="25"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3877,33 +3895,33 @@
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="46" t="s">
-        <v>40</v>
+      <c r="A66" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="C67" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="D67" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="25"/>
       <c r="B68" s="35"/>
-      <c r="C68" s="45">
-        <v>0</v>
-      </c>
-      <c r="D68" s="45">
+      <c r="C68" s="59">
+        <v>0</v>
+      </c>
+      <c r="D68" s="59">
         <v>0</v>
       </c>
     </row>
@@ -3933,7 +3951,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="12"/>
@@ -3941,107 +3959,107 @@
     </row>
     <row r="74" spans="1:7" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="30" t="s">
+      <c r="D74" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>48</v>
       </c>
       <c r="F74" s="21"/>
     </row>
     <row r="75" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="28"/>
-      <c r="B75" s="37">
-        <v>0</v>
-      </c>
-      <c r="C75" s="37">
-        <v>0</v>
-      </c>
-      <c r="D75" s="37">
+      <c r="B75" s="57">
+        <v>0</v>
+      </c>
+      <c r="C75" s="57">
+        <v>0</v>
+      </c>
+      <c r="D75" s="57">
         <v>0</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="27"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="43"/>
+      <c r="G76" s="41"/>
     </row>
     <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="27"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="43"/>
+      <c r="G77" s="41"/>
     </row>
     <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="27"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="43"/>
+      <c r="G78" s="41"/>
     </row>
     <row r="79" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="27"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="43"/>
+      <c r="G79" s="41"/>
     </row>
     <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="43"/>
+      <c r="G80" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="45" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="46" t="s">
         <v>51</v>
-      </c>
-      <c r="B85" s="48" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="25"/>
-      <c r="B86" s="45">
+      <c r="B86" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="25"/>
-      <c r="B87" s="45"/>
+      <c r="B87" s="43"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="25"/>
@@ -4052,146 +4070,146 @@
       <c r="B89" s="36"/>
     </row>
     <row r="91" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="46" t="s">
-        <v>53</v>
+      <c r="A91" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:7" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B92" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="F92" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>56</v>
       </c>
       <c r="G92" s="16"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="25"/>
-      <c r="B93" s="37">
-        <v>0</v>
-      </c>
-      <c r="C93" s="37">
-        <v>0</v>
-      </c>
-      <c r="D93" s="37">
-        <v>0</v>
-      </c>
-      <c r="E93" s="50"/>
+      <c r="B93" s="57">
+        <v>0</v>
+      </c>
+      <c r="C93" s="57">
+        <v>0</v>
+      </c>
+      <c r="D93" s="57">
+        <v>0</v>
+      </c>
+      <c r="E93" s="48"/>
       <c r="F93" s="25"/>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="25"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="50"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="48"/>
       <c r="F94" s="25"/>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="25"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="50"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="48"/>
       <c r="F95" s="25"/>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="25"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="50"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="48"/>
       <c r="F96" s="25"/>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="25"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="50"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="48"/>
       <c r="F97" s="25"/>
       <c r="G97" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
-        <v>57</v>
+      <c r="A99" s="45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E100" s="34" t="s">
+      <c r="F100" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F100" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="25"/>
-      <c r="B101" s="37">
-        <v>0</v>
-      </c>
-      <c r="C101" s="37">
-        <v>0</v>
-      </c>
-      <c r="D101" s="37">
-        <v>0</v>
-      </c>
-      <c r="E101" s="50"/>
+      <c r="B101" s="57">
+        <v>0</v>
+      </c>
+      <c r="C101" s="57">
+        <v>0</v>
+      </c>
+      <c r="D101" s="57">
+        <v>0</v>
+      </c>
+      <c r="E101" s="48"/>
       <c r="F101" s="25"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="25"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="50"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="48"/>
       <c r="F102" s="25"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="25"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="50"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="48"/>
       <c r="F103" s="25"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="25"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="50"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="48"/>
       <c r="F104" s="25"/>
     </row>
   </sheetData>
@@ -4210,8 +4228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4226,22 +4244,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>58</v>
+      <c r="A1" s="50" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+      <c r="A4" s="53">
         <v>42095</v>
       </c>
     </row>
@@ -4259,36 +4277,36 @@
         <v>0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="51">
         <v>60000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>65</v>
-      </c>
       <c r="B11" s="1">
-        <v>70000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -4296,7 +4314,7 @@
     </row>
     <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -4304,7 +4322,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -4319,16 +4337,16 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
+      <c r="A16" s="39" t="s">
+        <v>69</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -4336,15 +4354,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>4000000</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -4352,7 +4368,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -4360,32 +4376,32 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="54">
+        <v>4</v>
+      </c>
+      <c r="B21" s="52">
         <f>SUM(B9:B20)</f>
-        <v>4330000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="56">
+        <v>6</v>
+      </c>
+      <c r="B24" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -4393,7 +4409,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -4401,7 +4417,7 @@
     </row>
     <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -4409,7 +4425,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -4417,7 +4433,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -4425,29 +4441,29 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="57">
+        <v>9</v>
+      </c>
+      <c r="B30" s="55">
         <f>SUM(B24:B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="58">
+        <v>10</v>
+      </c>
+      <c r="B32" s="56">
         <f>(B21-B30)</f>
-        <v>4330000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -4455,21 +4471,21 @@
       <c r="C39" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>19</v>
+      <c r="A41" s="50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
-        <v>28</v>
+      <c r="A44" s="49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -4483,7 +4499,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4497,7 +4513,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4505,25 +4521,25 @@
     </row>
     <row r="50" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="C50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="E50" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="G50" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4531,14 +4547,14 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="25"/>
-      <c r="B51" s="37">
-        <v>0</v>
-      </c>
-      <c r="C51" s="37">
+      <c r="B51" s="57">
+        <v>0</v>
+      </c>
+      <c r="C51" s="57">
         <v>0</v>
       </c>
       <c r="D51" s="27"/>
-      <c r="E51" s="37">
+      <c r="E51" s="57">
         <v>0</v>
       </c>
       <c r="F51" s="25"/>
@@ -4549,10 +4565,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="25"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="25"/>
-      <c r="E52" s="38"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="3"/>
@@ -4561,10 +4577,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="25"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="25"/>
-      <c r="E53" s="38"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="3"/>
@@ -4573,10 +4589,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="37"/>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="3"/>
@@ -4585,10 +4601,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="25"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="25"/>
-      <c r="E55" s="38"/>
+      <c r="E55" s="37"/>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="3"/>
@@ -4597,10 +4613,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="25"/>
-      <c r="E56" s="38"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="3"/>
@@ -4613,68 +4629,68 @@
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
-        <v>39</v>
+      <c r="A58" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:10" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="C59" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="33" t="s">
+      <c r="E59" s="33" t="s">
         <v>15</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>16</v>
       </c>
       <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="39">
-        <v>0</v>
-      </c>
-      <c r="D60" s="39">
-        <v>0</v>
-      </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="41"/>
+      <c r="C60" s="58">
+        <v>0</v>
+      </c>
+      <c r="D60" s="58">
+        <v>0</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="39"/>
     </row>
     <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
       <c r="B61" s="25"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="25"/>
       <c r="B62" s="25"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
       <c r="B63" s="25"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="25"/>
       <c r="B64" s="25"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -4683,33 +4699,33 @@
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="46" t="s">
-        <v>40</v>
+      <c r="A66" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="C67" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="D67" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="25"/>
       <c r="B68" s="35"/>
-      <c r="C68" s="45">
-        <v>0</v>
-      </c>
-      <c r="D68" s="45">
+      <c r="C68" s="59">
+        <v>0</v>
+      </c>
+      <c r="D68" s="59">
         <v>0</v>
       </c>
     </row>
@@ -4739,115 +4755,115 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="12"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="30" t="s">
+      <c r="D74" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>48</v>
       </c>
       <c r="F74" s="21"/>
     </row>
     <row r="75" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="28"/>
-      <c r="B75" s="37">
-        <v>0</v>
-      </c>
-      <c r="C75" s="37">
-        <v>0</v>
-      </c>
-      <c r="D75" s="37">
+      <c r="B75" s="57">
+        <v>0</v>
+      </c>
+      <c r="C75" s="57">
+        <v>0</v>
+      </c>
+      <c r="D75" s="57">
         <v>0</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="27"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="43"/>
+      <c r="G76" s="41"/>
     </row>
     <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="27"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="43"/>
+      <c r="G77" s="41"/>
     </row>
     <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="27"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="43"/>
+      <c r="G78" s="41"/>
     </row>
     <row r="79" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="27"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="43"/>
+      <c r="G79" s="41"/>
     </row>
     <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="43"/>
+      <c r="G80" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="45" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="46" t="s">
         <v>51</v>
-      </c>
-      <c r="B85" s="48" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="25"/>
-      <c r="B86" s="45">
+      <c r="B86" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="25"/>
-      <c r="B87" s="45"/>
+      <c r="B87" s="43"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="25"/>
@@ -4858,146 +4874,146 @@
       <c r="B89" s="36"/>
     </row>
     <row r="91" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="46" t="s">
-        <v>53</v>
+      <c r="A91" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:7" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B92" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="F92" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>56</v>
       </c>
       <c r="G92" s="16"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="25"/>
-      <c r="B93" s="37">
-        <v>0</v>
-      </c>
-      <c r="C93" s="37">
-        <v>0</v>
-      </c>
-      <c r="D93" s="37">
-        <v>0</v>
-      </c>
-      <c r="E93" s="50"/>
+      <c r="B93" s="57">
+        <v>0</v>
+      </c>
+      <c r="C93" s="57">
+        <v>0</v>
+      </c>
+      <c r="D93" s="57">
+        <v>0</v>
+      </c>
+      <c r="E93" s="48"/>
       <c r="F93" s="25"/>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="25"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="50"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="48"/>
       <c r="F94" s="25"/>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="25"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="50"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="48"/>
       <c r="F95" s="25"/>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="25"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="50"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="48"/>
       <c r="F96" s="25"/>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="25"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="50"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="48"/>
       <c r="F97" s="25"/>
       <c r="G97" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
-        <v>57</v>
+      <c r="A99" s="45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E100" s="34" t="s">
+      <c r="F100" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="F100" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="25"/>
-      <c r="B101" s="37">
-        <v>0</v>
-      </c>
-      <c r="C101" s="37">
-        <v>0</v>
-      </c>
-      <c r="D101" s="37">
-        <v>0</v>
-      </c>
-      <c r="E101" s="50"/>
+      <c r="B101" s="57">
+        <v>0</v>
+      </c>
+      <c r="C101" s="57">
+        <v>0</v>
+      </c>
+      <c r="D101" s="57">
+        <v>0</v>
+      </c>
+      <c r="E101" s="48"/>
       <c r="F101" s="25"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="25"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="50"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="48"/>
       <c r="F102" s="25"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="25"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="50"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="48"/>
       <c r="F103" s="25"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="25"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="50"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="48"/>
       <c r="F104" s="25"/>
     </row>
   </sheetData>

</xml_diff>